<commit_message>
Structured project directory and fixed all checkstyle warnings
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog.xlsx
+++ b/documentation/Sprint Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/destiny/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/destiny/Desktop/CS3211DiscountFinder/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9FA0D57-2AD5-CF4A-B751-D897A38086E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE9AD72-1B4C-E147-BD94-860925B58752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="13560" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -97,6 +97,21 @@
   </si>
   <si>
     <t>Implement Clear Filters button functionality</t>
+  </si>
+  <si>
+    <t>Implement Favorite Seller functionality</t>
+  </si>
+  <si>
+    <t>Favorite Seller</t>
+  </si>
+  <si>
+    <t>Implement Radion Button Functionality for filter</t>
+  </si>
+  <si>
+    <t>Destiny</t>
+  </si>
+  <si>
+    <t>Actual</t>
   </si>
 </sst>
 </file>
@@ -120,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +160,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -158,12 +179,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -449,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7020883B-3029-4319-B006-C2C3BA3C5B2B}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -461,23 +486,27 @@
     <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -490,8 +519,11 @@
       <c r="D2" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -504,8 +536,11 @@
       <c r="D3" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -518,8 +553,11 @@
       <c r="D4" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -532,8 +570,11 @@
       <c r="D5" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -546,8 +587,11 @@
       <c r="D6" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -560,8 +604,11 @@
       <c r="D7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -574,8 +621,11 @@
       <c r="D8" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -588,21 +638,58 @@
       <c r="D9" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="2">
-        <f>SUM(D2:D9)</f>
+      <c r="B12" s="7"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="2">
+        <f>SUM(D2:D10)</f>
         <v>6.75</v>
+      </c>
+      <c r="E12" s="2">
+        <f>SUM(E2:E11)</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>